<commit_message>
Modificaciones finales automatización de pruebas con Selenium y cucumber
</commit_message>
<xml_diff>
--- a/productosSportLine.xlsx
+++ b/productosSportLine.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,27 +19,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>NombreProducto</t>
   </si>
   <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Mujer&gt;Calzado</t>
-  </si>
-  <si>
-    <t>Air Zoom Vomero 14</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Nike</t>
-  </si>
-  <si>
-    <t>$654.950</t>
+    <t>Advanced Trainette</t>
+  </si>
+  <si>
+    <t>Reebok Hiit Tr Dynred</t>
+  </si>
+  <si>
+    <t>Downshifter 9</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Lebron Witness 4</t>
+  </si>
+  <si>
+    <t>Air Max 720</t>
+  </si>
+  <si>
+    <t>Court Borough Low 2</t>
+  </si>
+  <si>
+    <t>Niños</t>
   </si>
 </sst>
 </file>
@@ -76,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,50 +417,64 @@
     <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>